<commit_message>
'Slow' Floor Materials added
</commit_message>
<xml_diff>
--- a/SAWZE_Documentation/Last Mile/unic_lvl_assts_brainstorm.xlsx
+++ b/SAWZE_Documentation/Last Mile/unic_lvl_assts_brainstorm.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>from</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Playstation, Game CDs, Game Posters (fake games), Arcade Game Consol</t>
+  </si>
+  <si>
+    <t>Tobi</t>
+  </si>
+  <si>
+    <t>Murder</t>
+  </si>
+  <si>
+    <t>Kreideleichen und so(Amon hats reingeschrieben, Tobi bitte ergänzen)</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,9 +468,15 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>

</xml_diff>